<commit_message>
kti tmp fixed + minor fixes added
</commit_message>
<xml_diff>
--- a/templates/Invoice_KTI_Discharge.xlsx
+++ b/templates/Invoice_KTI_Discharge.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C86A47-DD71-4935-9475-766742E01EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B0F367-4E38-4DDF-B553-46EAA75A0C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="KTI_LOGO">Invoice_KTI!$B$2</definedName>
     <definedName name="KTI_LOGO_п">Invoice_KTI!$B$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice_KTI!$A$1:$I$65</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice_KTI!$A$1:$I$66</definedName>
     <definedName name="Инвойс_всего">Invoice_KTI!#REF!</definedName>
     <definedName name="Инвойс_всего_п">Invoice_KTI!#REF!</definedName>
     <definedName name="Инвойс_выгрузка_дата">Invoice_KTI!$C$17</definedName>
@@ -34,7 +34,7 @@
     <definedName name="Инвойс_номер">Invoice_KTI!$E$8</definedName>
     <definedName name="Инвойс_номер_п">Invoice_KTI!$E$41</definedName>
     <definedName name="Инвойс_п_граница">Invoice_KTI!$B$33</definedName>
-    <definedName name="Инвойс_печать">Invoice_KTI!$B$64</definedName>
+    <definedName name="Инвойс_печать">Invoice_KTI!$B$66</definedName>
     <definedName name="Инвойс_соглашение">Invoice_KTI!$C$21</definedName>
     <definedName name="Инвойс_соглашение_п">Invoice_KTI!$C$53</definedName>
     <definedName name="Инвойс_таблица_заголовок">Invoice_KTI!$B$24</definedName>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
   <si>
     <t xml:space="preserve">PROFORMA INVOICE No. </t>
   </si>
@@ -115,9 +115,6 @@
     <t>Request for payment for discharging operations</t>
   </si>
   <si>
-    <t xml:space="preserve"> DISCHARGING CHARGE</t>
-  </si>
-  <si>
     <t>Storage Servise contract № 410/33961105/0012 from February, 01, 2022</t>
   </si>
   <si>
@@ -230,6 +227,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Discharging Charge</t>
   </si>
 </sst>
 </file>
@@ -238,9 +238,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-809]d\ mmmm\ yyyy;@"/>
-    <numFmt numFmtId="170" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
+    <numFmt numFmtId="165" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
@@ -298,12 +298,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="204"/>
@@ -389,7 +383,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -492,9 +486,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -503,42 +495,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -552,12 +520,15 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -565,34 +536,31 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -602,21 +570,15 @@
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -624,57 +586,48 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="170" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1003,8 +956,8 @@
   </sheetPr>
   <dimension ref="B1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A48" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E68" sqref="E68"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1844,8 +1797,8 @@
   <sheetData>
     <row r="1" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="56" t="s">
-        <v>55</v>
+      <c r="B2" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>13</v>
@@ -1859,7 +1812,7 @@
     </row>
     <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="14"/>
     </row>
@@ -1873,17 +1826,17 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1894,7 +1847,7 @@
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
@@ -1910,12 +1863,12 @@
         <v>2</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="H10" s="40">
+        <v>50</v>
+      </c>
+      <c r="H10" s="45">
         <v>45079</v>
       </c>
-      <c r="I10" s="40"/>
+      <c r="I10" s="45"/>
     </row>
     <row r="11" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
@@ -1926,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
@@ -1970,7 +1923,7 @@
         <v>6</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D17" s="8"/>
       <c r="E17" s="18"/>
@@ -1987,7 +1940,7 @@
         <v>7</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
@@ -2001,10 +1954,10 @@
     </row>
     <row r="21" spans="2:9" ht="31.9" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B21" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -2018,33 +1971,33 @@
     </row>
     <row r="23" spans="2:9" ht="10.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="24" spans="2:9" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52"/>
-      <c r="G24" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="34" t="s">
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="51" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="51" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="50.65" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C25" s="47"/>
-      <c r="D25" s="47"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="48"/>
-      <c r="G25" s="38" t="s">
+      <c r="B25" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="39"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="H25" s="35" t="s">
         <v>53</v>
-      </c>
-      <c r="H25" s="37" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2076,17 +2029,17 @@
       <c r="H31" s="19"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="G32" s="46"/>
+      <c r="G32" s="38"/>
     </row>
     <row r="33" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="11.35" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:9" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C35" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -2097,7 +2050,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C36" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2107,50 +2060,50 @@
       <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B37" s="56" t="s">
-        <v>55</v>
+      <c r="B37" s="44" t="s">
+        <v>54</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C38" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
+      <c r="G38" s="50"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B39" s="15"/>
-      <c r="C39" s="44" t="s">
+      <c r="C39" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49"/>
+      <c r="F39" s="49"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
       <c r="I39" s="15"/>
     </row>
     <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
@@ -2158,19 +2111,19 @@
       <c r="I41" s="17"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="G42" s="54" t="s">
-        <v>52</v>
-      </c>
-      <c r="H42" s="55">
+      <c r="G42" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="H42" s="43">
         <v>45033</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I43" s="33"/>
     </row>
@@ -2180,10 +2133,10 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B45" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -2204,10 +2157,10 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B47" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -2218,10 +2171,10 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B49" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>39</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="18"/>
@@ -2235,10 +2188,10 @@
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="18"/>
@@ -2252,10 +2205,10 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B53" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
@@ -2277,34 +2230,34 @@
       <c r="H55" s="31"/>
     </row>
     <row r="56" spans="2:9" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B56" s="39" t="s">
+      <c r="B56" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="37"/>
+      <c r="D56" s="37"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="37"/>
+      <c r="G56" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="39"/>
-      <c r="D56" s="39"/>
-      <c r="E56" s="39"/>
-      <c r="F56" s="39"/>
-      <c r="G56" s="35" t="s">
+      <c r="H56" s="34" t="s">
         <v>49</v>
-      </c>
-      <c r="H56" s="35" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="57" spans="2:9" s="28" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C57" s="29"/>
       <c r="D57" s="29"/>
       <c r="E57" s="29"/>
-      <c r="F57" s="49"/>
-      <c r="G57" s="53"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="41"/>
       <c r="H57" s="30"/>
     </row>
     <row r="58" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -2323,12 +2276,17 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G63" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G63" s="20" t="s">
-        <v>45</v>
-      </c>
       <c r="H63" s="19"/>
+    </row>
+    <row r="66" spans="2:2" ht="1.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.4">
       <c r="B81" s="23"/>
@@ -2340,22 +2298,21 @@
       <c r="H81" s="27"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B82" s="43"/>
-      <c r="C82" s="43"/>
-      <c r="D82" s="43"/>
-      <c r="E82" s="43"/>
-      <c r="F82" s="43"/>
-      <c r="G82" s="43"/>
-      <c r="H82" s="43"/>
+      <c r="B82" s="48"/>
+      <c r="C82" s="48"/>
+      <c r="D82" s="48"/>
+      <c r="E82" s="48"/>
+      <c r="F82" s="48"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="48"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="B82:H82"/>
-    <mergeCell ref="B24:F24"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="G37:H37"/>

</xml_diff>

<commit_message>
invoice kti tmp fixed, dt module in progress
</commit_message>
<xml_diff>
--- a/templates/Invoice_KTI_Discharge.xlsx
+++ b/templates/Invoice_KTI_Discharge.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B0F367-4E38-4DDF-B553-46EAA75A0C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C8680D-6BBE-409B-9A7F-2A73F197C4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
@@ -33,6 +33,8 @@
     <definedName name="Инвойс_массив_п">Invoice_KTI!$B$57</definedName>
     <definedName name="Инвойс_номер">Invoice_KTI!$E$8</definedName>
     <definedName name="Инвойс_номер_п">Invoice_KTI!$E$41</definedName>
+    <definedName name="Инвойс_объект">Invoice_KTI!$C$14</definedName>
+    <definedName name="Инвойс_объект_п">Invoice_KTI!$C$47</definedName>
     <definedName name="Инвойс_п_граница">Invoice_KTI!$B$33</definedName>
     <definedName name="Инвойс_печать">Invoice_KTI!$B$66</definedName>
     <definedName name="Инвойс_соглашение">Invoice_KTI!$C$21</definedName>
@@ -145,12 +147,6 @@
     <t>7, Чунг-Джанг-даэро, Юнг-Гу, Пусан, Республика Корея, (Юнганг-Донг-4га, КЁБО Б/Д 2Ф, 3Ф)</t>
   </si>
   <si>
-    <t>Тел.: 600-7475</t>
-  </si>
-  <si>
-    <t>Факс: 231-5222</t>
-  </si>
-  <si>
     <t xml:space="preserve">ПРОФОРМА ИНВОЙС № </t>
   </si>
   <si>
@@ -230,6 +226,12 @@
   </si>
   <si>
     <t>Discharging Charge</t>
+  </si>
+  <si>
+    <t>Тел.: 466-1401</t>
+  </si>
+  <si>
+    <t>Факс: 466-1404</t>
   </si>
 </sst>
 </file>
@@ -610,6 +612,9 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -625,9 +630,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -956,8 +958,8 @@
   </sheetPr>
   <dimension ref="B1:I82"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A6" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1798,7 +1800,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="44" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>13</v>
@@ -1826,17 +1828,17 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="46"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="48"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1863,12 +1865,12 @@
         <v>2</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="45">
+        <v>48</v>
+      </c>
+      <c r="H10" s="46">
         <v>45079</v>
       </c>
-      <c r="I10" s="45"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="11" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
@@ -1978,10 +1980,10 @@
       <c r="D24" s="37"/>
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
-      <c r="G24" s="51" t="s">
-        <v>55</v>
-      </c>
-      <c r="H24" s="51" t="s">
+      <c r="G24" s="45" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="45" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1994,10 +1996,10 @@
       <c r="E25" s="39"/>
       <c r="F25" s="40"/>
       <c r="G25" s="36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2033,7 +2035,7 @@
     </row>
     <row r="33" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="11.35" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2061,49 +2063,49 @@
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B37" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
+      <c r="G37" s="51"/>
+      <c r="H37" s="51"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C38" s="4" t="s">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="50"/>
+      <c r="G38" s="51"/>
+      <c r="H38" s="51"/>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B39" s="15"/>
-      <c r="C39" s="49" t="s">
+      <c r="C39" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
       <c r="I39" s="15"/>
     </row>
     <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
@@ -2112,7 +2114,7 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.4">
       <c r="G42" s="42" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H42" s="43">
         <v>45033</v>
@@ -2120,10 +2122,10 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I43" s="33"/>
     </row>
@@ -2133,10 +2135,10 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B45" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -2157,10 +2159,10 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B47" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -2171,10 +2173,10 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B49" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C49" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="18"/>
@@ -2188,10 +2190,10 @@
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B51" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="18"/>
@@ -2205,10 +2207,10 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B53" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
@@ -2231,22 +2233,22 @@
     </row>
     <row r="56" spans="2:9" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B56" s="37" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
       <c r="G56" s="34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="57" spans="2:9" s="28" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C57" s="29"/>
       <c r="D57" s="29"/>
@@ -2257,7 +2259,7 @@
     </row>
     <row r="58" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -2276,16 +2278,16 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H63" s="19"/>
     </row>
     <row r="66" spans="2:2" ht="1.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.4">
@@ -2298,13 +2300,13 @@
       <c r="H81" s="27"/>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B82" s="48"/>
-      <c r="C82" s="48"/>
-      <c r="D82" s="48"/>
-      <c r="E82" s="48"/>
-      <c r="F82" s="48"/>
-      <c r="G82" s="48"/>
-      <c r="H82" s="48"/>
+      <c r="B82" s="49"/>
+      <c r="C82" s="49"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="49"/>
+      <c r="F82" s="49"/>
+      <c r="G82" s="49"/>
+      <c r="H82" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
KTI Invoice tmp updated
</commit_message>
<xml_diff>
--- a/templates/Invoice_KTI_Discharge.xlsx
+++ b/templates/Invoice_KTI_Discharge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C8680D-6BBE-409B-9A7F-2A73F197C4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FABC39E-2FD2-4269-A06E-1F033818AA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16395" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
+    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16035" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_KTI" sheetId="70" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="KTI_LOGO">Invoice_KTI!$B$2</definedName>
     <definedName name="KTI_LOGO_п">Invoice_KTI!$B$37</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice_KTI!$A$1:$I$66</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Invoice_KTI!$A$1:$I$71</definedName>
     <definedName name="Инвойс_всего">Invoice_KTI!#REF!</definedName>
     <definedName name="Инвойс_всего_п">Invoice_KTI!#REF!</definedName>
     <definedName name="Инвойс_выгрузка_дата">Invoice_KTI!$C$17</definedName>
@@ -36,7 +36,9 @@
     <definedName name="Инвойс_объект">Invoice_KTI!$C$14</definedName>
     <definedName name="Инвойс_объект_п">Invoice_KTI!$C$47</definedName>
     <definedName name="Инвойс_п_граница">Invoice_KTI!$B$33</definedName>
-    <definedName name="Инвойс_печать">Invoice_KTI!$B$66</definedName>
+    <definedName name="Инвойс_перевод_конец_п">Invoice_KTI!$B$69</definedName>
+    <definedName name="Инвойс_перевод_старт_п">Invoice_KTI!$B$66</definedName>
+    <definedName name="Инвойс_печать">Invoice_KTI!$B$71</definedName>
     <definedName name="Инвойс_соглашение">Invoice_KTI!$C$21</definedName>
     <definedName name="Инвойс_соглашение_п">Invoice_KTI!$C$53</definedName>
     <definedName name="Инвойс_таблица_заголовок">Invoice_KTI!$B$24</definedName>
@@ -64,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
   <si>
     <t xml:space="preserve">PROFORMA INVOICE No. </t>
   </si>
@@ -232,6 +234,15 @@
   </si>
   <si>
     <t>Факс: 466-1404</t>
+  </si>
+  <si>
+    <t>Перевод осуществлен переводчиком Таранушко Натальей Ивановной,</t>
+  </si>
+  <si>
+    <t>Диплом ВСВ № 1853344, выдан 20.06.2006 г., Северный Международный Университет, г. Магадан</t>
+  </si>
+  <si>
+    <t>Подпись Таранушко Н. И.</t>
   </si>
 </sst>
 </file>
@@ -242,11 +253,19 @@
     <numFmt numFmtId="164" formatCode="[$-809]d\ mmmm\ yyyy;@"/>
     <numFmt numFmtId="165" formatCode="[$-FC19]dd\ mmmm\ yyyy\ \г\.;@"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="돋움"/>
       <charset val="129"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -376,6 +395,12 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -498,39 +523,37 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="4" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -538,105 +561,113 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="7" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="4" xr:uid="{156BA76C-6742-4160-954A-D0558E5179DE}"/>
     <cellStyle name="Обычный 3" xfId="6" xr:uid="{9614D98E-2F78-43A7-BC02-E013ED4FACC0}"/>
     <cellStyle name="Обычный 5" xfId="7" xr:uid="{9CE7B968-839A-4186-BEA9-9E0047086641}"/>
+    <cellStyle name="Обычный 5 2 2 2" xfId="8" xr:uid="{8918AC56-F3E0-4348-A855-A10C3EC07786}"/>
     <cellStyle name="Обычный_Лист1 2_Hong-Kong Снабжение 2" xfId="2" xr:uid="{61A0CD1A-29D1-4416-93F0-A4CB118EA012}"/>
     <cellStyle name="Обычный_Лист1 3 2" xfId="3" xr:uid="{BD549A16-FCCA-4D8F-90BF-33FE4372EC1A}"/>
     <cellStyle name="Обычный_Лист1 4" xfId="5" xr:uid="{CE28593A-A524-4A7B-8D76-7CEA3E5636EB}"/>
@@ -956,10 +987,10 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:I82"/>
+  <dimension ref="B1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A27" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A45" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1828,17 +1859,17 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="48"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="48"/>
+      <c r="H6" s="48"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1867,10 +1898,10 @@
       <c r="G10" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="H10" s="46">
+      <c r="H10" s="47">
         <v>45079</v>
       </c>
-      <c r="I10" s="46"/>
+      <c r="I10" s="47"/>
     </row>
     <row r="11" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
@@ -2062,17 +2093,15 @@
       <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="B37" s="44" t="s">
-        <v>52</v>
-      </c>
+      <c r="B37" s="44"/>
       <c r="C37" s="4" t="s">
         <v>54</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.4">
@@ -2082,20 +2111,20 @@
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="51"/>
-      <c r="H38" s="51"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B39" s="15"/>
-      <c r="C39" s="50" t="s">
+      <c r="C39" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="50"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="50"/>
-      <c r="G39" s="47"/>
-      <c r="H39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="48"/>
       <c r="I39" s="15"/>
     </row>
     <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.4">
@@ -2285,28 +2314,70 @@
       </c>
       <c r="H63" s="19"/>
     </row>
-    <row r="66" spans="2:2" ht="1.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="6" t="s">
+    <row r="65" spans="2:8" ht="89.35" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B66" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="C66" s="53"/>
+      <c r="D66" s="53"/>
+      <c r="E66" s="53"/>
+      <c r="F66" s="53"/>
+      <c r="G66" s="53"/>
+      <c r="H66" s="53"/>
+    </row>
+    <row r="67" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B67" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="C67" s="53"/>
+      <c r="D67" s="53"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="53"/>
+      <c r="G67" s="53"/>
+      <c r="H67" s="53"/>
+    </row>
+    <row r="68" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B68" s="46"/>
+      <c r="C68" s="46"/>
+      <c r="D68" s="46"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+    </row>
+    <row r="69" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B69" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="53"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="53"/>
+      <c r="G69" s="53"/>
+      <c r="H69" s="53"/>
+    </row>
+    <row r="71" spans="2:8" ht="3.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B71" s="6" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B81" s="23"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="25"/>
-      <c r="F81" s="26"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="27"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B82" s="49"/>
-      <c r="C82" s="49"/>
-      <c r="D82" s="49"/>
-      <c r="E82" s="49"/>
-      <c r="F82" s="49"/>
-      <c r="G82" s="49"/>
-      <c r="H82" s="49"/>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B86" s="23"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="25"/>
+      <c r="E86" s="25"/>
+      <c r="F86" s="26"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="27"/>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="B87" s="50"/>
+      <c r="C87" s="50"/>
+      <c r="D87" s="50"/>
+      <c r="E87" s="50"/>
+      <c r="F87" s="50"/>
+      <c r="G87" s="50"/>
+      <c r="H87" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -2314,14 +2385,14 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="G6:H6"/>
-    <mergeCell ref="B82:H82"/>
+    <mergeCell ref="B87:H87"/>
     <mergeCell ref="C39:F39"/>
     <mergeCell ref="G39:H39"/>
     <mergeCell ref="G37:H37"/>
     <mergeCell ref="G38:H38"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0" top="0" bottom="0" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="92" fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="90" fitToHeight="0" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
kti company tmp updated
</commit_message>
<xml_diff>
--- a/templates/Invoice_KTI_Discharge.xlsx
+++ b/templates/Invoice_KTI_Discharge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FABC39E-2FD2-4269-A06E-1F033818AA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25529047-EDBC-4ACE-AAB6-2C2B71AAE6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="16035" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15436" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_KTI" sheetId="70" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="Инвойс_выгрузка_дата">Invoice_KTI!$C$17</definedName>
     <definedName name="Инвойс_выгрузка_дата_п">Invoice_KTI!$C$49</definedName>
     <definedName name="Инвойс_дата">Invoice_KTI!$H$10</definedName>
-    <definedName name="Инвойс_дата_п">Invoice_KTI!$H$42</definedName>
+    <definedName name="Инвойс_дата_п">Invoice_KTI!$H$43</definedName>
     <definedName name="Инвойс_компания">Invoice_KTI!$C$10</definedName>
     <definedName name="Инвойс_компания_п">Invoice_KTI!$C$43</definedName>
     <definedName name="Инвойс_контракт">Invoice_KTI!$C$12</definedName>
@@ -143,9 +143,6 @@
     <t>Supplementary Agreement</t>
   </si>
   <si>
-    <t>KTI Компани Лимитед</t>
-  </si>
-  <si>
     <t>7, Чунг-Джанг-даэро, Юнг-Гу, Пусан, Республика Корея, (Юнганг-Донг-4га, КЁБО Б/Д 2Ф, 3Ф)</t>
   </si>
   <si>
@@ -188,9 +185,6 @@
     <t>СРТМ "Си Хантер"  Икра минтая мороженая (MSC)</t>
   </si>
   <si>
-    <t>Принято и подтверждено</t>
-  </si>
-  <si>
     <t>Покупатель</t>
   </si>
   <si>
@@ -243,6 +237,12 @@
   </si>
   <si>
     <t>Подпись Таранушко Н. И.</t>
+  </si>
+  <si>
+    <t>КТИ Компани Лимитед</t>
+  </si>
+  <si>
+    <t>Принял и подтвердил</t>
   </si>
 </sst>
 </file>
@@ -644,6 +644,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -660,7 +661,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -989,8 +989,8 @@
   </sheetPr>
   <dimension ref="B1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A45" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -1831,7 +1831,7 @@
     <row r="1" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="2:9" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B2" s="44" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>13</v>
@@ -1859,17 +1859,17 @@
       <c r="C5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
       <c r="I5" s="15"/>
     </row>
     <row r="6" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="15"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="48"/>
-      <c r="H6" s="48"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
       <c r="I6" s="15"/>
     </row>
     <row r="7" spans="2:9" ht="9.6" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1896,12 +1896,12 @@
         <v>2</v>
       </c>
       <c r="G10" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="H10" s="47">
+        <v>46</v>
+      </c>
+      <c r="H10" s="48">
         <v>45079</v>
       </c>
-      <c r="I10" s="47"/>
+      <c r="I10" s="48"/>
     </row>
     <row r="11" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B11" s="3"/>
@@ -2012,7 +2012,7 @@
       <c r="E24" s="37"/>
       <c r="F24" s="37"/>
       <c r="G24" s="45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H24" s="45" t="s">
         <v>9</v>
@@ -2027,10 +2027,10 @@
       <c r="E25" s="39"/>
       <c r="F25" s="40"/>
       <c r="G25" s="36" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -2066,13 +2066,13 @@
     </row>
     <row r="33" spans="2:9" ht="4.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B33" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="11.35" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:9" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C35" s="11" t="s">
-        <v>25</v>
+        <v>57</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -2083,7 +2083,7 @@
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C36" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -2095,66 +2095,64 @@
     <row r="37" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B37" s="44"/>
       <c r="C37" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="53"/>
       <c r="I37" s="22"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.4">
       <c r="C38" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
       <c r="I38" s="22"/>
     </row>
     <row r="39" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B39" s="15"/>
-      <c r="C39" s="51" t="s">
+      <c r="C39" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="D39" s="51"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
       <c r="I39" s="15"/>
     </row>
     <row r="41" spans="2:9" ht="15" x14ac:dyDescent="0.4">
       <c r="B41" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F41" s="16"/>
       <c r="G41" s="17"/>
       <c r="H41" s="17"/>
       <c r="I41" s="17"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.4">
-      <c r="G42" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="H42" s="43">
-        <v>45033</v>
-      </c>
-    </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>30</v>
+      <c r="G43" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H43" s="43">
+        <v>45033</v>
       </c>
       <c r="I43" s="33"/>
     </row>
@@ -2164,10 +2162,10 @@
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>32</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
@@ -2188,10 +2186,10 @@
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B47" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C47" s="5" t="s">
-        <v>34</v>
       </c>
       <c r="D47" s="18"/>
       <c r="E47" s="18"/>
@@ -2202,10 +2200,10 @@
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B49" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C49" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="C49" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="18"/>
@@ -2219,10 +2217,10 @@
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>38</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="18"/>
@@ -2236,10 +2234,10 @@
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B53" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D53" s="18"/>
       <c r="E53" s="18"/>
@@ -2262,22 +2260,22 @@
     </row>
     <row r="56" spans="2:9" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B56" s="37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C56" s="37"/>
       <c r="D56" s="37"/>
       <c r="E56" s="37"/>
       <c r="F56" s="37"/>
       <c r="G56" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H56" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="2:9" s="28" customFormat="1" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B57" s="29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C57" s="29"/>
       <c r="D57" s="29"/>
@@ -2288,7 +2286,7 @@
     </row>
     <row r="58" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="4" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -2307,35 +2305,35 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B63" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H63" s="19"/>
     </row>
     <row r="65" spans="2:8" ht="89.35" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="66" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B66" s="53" t="s">
-        <v>56</v>
-      </c>
-      <c r="C66" s="53"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="53"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="53"/>
+      <c r="B66" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C66" s="47"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="47"/>
+      <c r="G66" s="47"/>
+      <c r="H66" s="47"/>
     </row>
     <row r="67" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="53" t="s">
-        <v>57</v>
-      </c>
-      <c r="C67" s="53"/>
-      <c r="D67" s="53"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="53"/>
-      <c r="G67" s="53"/>
-      <c r="H67" s="53"/>
+      <c r="B67" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" s="47"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="47"/>
+      <c r="G67" s="47"/>
+      <c r="H67" s="47"/>
     </row>
     <row r="68" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B68" s="46"/>
@@ -2346,19 +2344,19 @@
       <c r="G68" s="46"/>
     </row>
     <row r="69" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="53" t="s">
-        <v>58</v>
-      </c>
-      <c r="C69" s="53"/>
-      <c r="D69" s="53"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="53"/>
-      <c r="G69" s="53"/>
-      <c r="H69" s="53"/>
+      <c r="B69" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C69" s="47"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="47"/>
+      <c r="G69" s="47"/>
+      <c r="H69" s="47"/>
     </row>
     <row r="71" spans="2:8" ht="3.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.4">
@@ -2371,13 +2369,13 @@
       <c r="H86" s="27"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.4">
-      <c r="B87" s="50"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="50"/>
-      <c r="F87" s="50"/>
-      <c r="G87" s="50"/>
-      <c r="H87" s="50"/>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="51"/>
+      <c r="E87" s="51"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
minor fixes on buhMail + invoiceKTISection updated, added translator select
</commit_message>
<xml_diff>
--- a/templates/Invoice_KTI_Discharge.xlsx
+++ b/templates/Invoice_KTI_Discharge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\papka\TSAddIn\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25529047-EDBC-4ACE-AAB6-2C2B71AAE6BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8FF5EF-6574-456F-940A-492AC56B002D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15436" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="27076" windowHeight="16636" tabRatio="896" xr2:uid="{A5E11D55-FD63-4C1B-A2BC-73BE53B894FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice_KTI" sheetId="70" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <definedName name="Инвойс_выгрузка_дата_п">Invoice_KTI!$C$49</definedName>
     <definedName name="Инвойс_дата">Invoice_KTI!$H$10</definedName>
     <definedName name="Инвойс_дата_п">Invoice_KTI!$H$43</definedName>
+    <definedName name="Инвойс_исполнитель_КИА">Invoice_KTI!$B$69</definedName>
+    <definedName name="Инвойс_исполнитель_ТНИ">Invoice_KTI!$B$67</definedName>
     <definedName name="Инвойс_компания">Invoice_KTI!$C$10</definedName>
     <definedName name="Инвойс_компания_п">Invoice_KTI!$C$43</definedName>
     <definedName name="Инвойс_контракт">Invoice_KTI!$C$12</definedName>
@@ -36,7 +38,7 @@
     <definedName name="Инвойс_объект">Invoice_KTI!$C$14</definedName>
     <definedName name="Инвойс_объект_п">Invoice_KTI!$C$47</definedName>
     <definedName name="Инвойс_п_граница">Invoice_KTI!$B$33</definedName>
-    <definedName name="Инвойс_перевод_конец_п">Invoice_KTI!$B$69</definedName>
+    <definedName name="Инвойс_перевод_конец_п">Invoice_KTI!$B$70</definedName>
     <definedName name="Инвойс_перевод_старт_п">Invoice_KTI!$B$66</definedName>
     <definedName name="Инвойс_печать">Invoice_KTI!$B$71</definedName>
     <definedName name="Инвойс_соглашение">Invoice_KTI!$C$21</definedName>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="58">
   <si>
     <t xml:space="preserve">PROFORMA INVOICE No. </t>
   </si>
@@ -230,19 +232,20 @@
     <t>Факс: 466-1404</t>
   </si>
   <si>
-    <t>Перевод осуществлен переводчиком Таранушко Натальей Ивановной,</t>
-  </si>
-  <si>
-    <t>Диплом ВСВ № 1853344, выдан 20.06.2006 г., Северный Международный Университет, г. Магадан</t>
-  </si>
-  <si>
-    <t>Подпись Таранушко Н. И.</t>
-  </si>
-  <si>
     <t>КТИ Компани Лимитед</t>
   </si>
   <si>
     <t>Принял и подтвердил</t>
+  </si>
+  <si>
+    <t>Перевод осуществлен переводчиком Таранушко Натальей Ивановной,
+Диплом ВСВ № 1853344, выдан 20.06.2006 г., Северный Международный Университет, г. Магадан
+Подпись Таранушко Н. И.</t>
+  </si>
+  <si>
+    <t>Перевод осуществлен переводчиком Ким Ириной Александровной
+Диплом № 1049080000632, выдан 26.06.2024 г., Северо-Восточный Государственный Университет, г. Магадан.
+Подпись Ким И. А.</t>
   </si>
 </sst>
 </file>
@@ -534,7 +537,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -660,6 +663,21 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -989,8 +1007,8 @@
   </sheetPr>
   <dimension ref="B1:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A56" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -2072,7 +2090,7 @@
     <row r="34" spans="2:9" ht="11.35" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="35" spans="2:9" ht="30.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="C35" s="11" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D35" s="11"/>
       <c r="E35" s="11"/>
@@ -2286,7 +2304,7 @@
     </row>
     <row r="58" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B58" s="4" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.4">
@@ -2312,10 +2330,10 @@
       </c>
       <c r="H63" s="19"/>
     </row>
-    <row r="65" spans="2:8" ht="89.35" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="66" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:8" ht="57.85" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="66" spans="2:8" ht="2.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B66" s="47" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C66" s="47"/>
       <c r="D66" s="47"/>
@@ -2324,37 +2342,42 @@
       <c r="G66" s="47"/>
       <c r="H66" s="47"/>
     </row>
-    <row r="67" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B67" s="47" t="s">
-        <v>55</v>
-      </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="47"/>
-      <c r="E67" s="47"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-      <c r="H67" s="47"/>
+    <row r="67" spans="2:8" s="55" customFormat="1" ht="72.849999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C67" s="56"/>
+      <c r="D67" s="56"/>
+      <c r="E67" s="56"/>
+      <c r="F67" s="56"/>
+      <c r="G67" s="56"/>
+      <c r="H67" s="54"/>
     </row>
     <row r="68" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B68" s="46"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="46"/>
       <c r="D68" s="46"/>
       <c r="E68" s="46"/>
       <c r="F68" s="46"/>
       <c r="G68" s="46"/>
     </row>
-    <row r="69" spans="2:8" ht="17.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B69" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C69" s="47"/>
-      <c r="D69" s="47"/>
-      <c r="E69" s="47"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
-      <c r="H69" s="47"/>
-    </row>
-    <row r="71" spans="2:8" ht="3.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="2:8" s="58" customFormat="1" ht="76.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="56" t="s">
+        <v>57</v>
+      </c>
+      <c r="C69" s="56"/>
+      <c r="D69" s="56"/>
+      <c r="E69" s="56"/>
+      <c r="F69" s="56"/>
+      <c r="G69" s="56"/>
+      <c r="H69" s="57"/>
+    </row>
+    <row r="70" spans="2:8" ht="3" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B70" s="47" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="20.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B71" s="6" t="s">
         <v>50</v>
       </c>

</xml_diff>